<commit_message>
Break out Equipment and Location changes
</commit_message>
<xml_diff>
--- a/cypress/fixtures/AnnexA5.xlsx
+++ b/cypress/fixtures/AnnexA5.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joero\Documents\GitHub\cypress-cucumber-example\cypress\fixtures\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A282CD-8BD2-4B2A-8D17-0C10ADF7BB3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="120" windowWidth="14340" windowHeight="3984"/>
+    <workbookView xWindow="-9960" yWindow="2535" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,9 +60,6 @@
     <t>W333</t>
   </si>
   <si>
-    <t>S2706 ASTUTE</t>
-  </si>
-  <si>
     <t>W333 200025601</t>
   </si>
   <si>
@@ -76,12 +79,15 @@
   </si>
   <si>
     <t>SCREW CAP</t>
+  </si>
+  <si>
+    <t>Sonar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -122,6 +128,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -170,7 +179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -203,9 +212,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -238,6 +264,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,24 +456,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B3" sqref="B3:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +493,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -470,18 +513,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -490,18 +533,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -510,18 +553,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -530,18 +573,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -556,24 +599,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>